<commit_message>
updated db name in xlsx
</commit_message>
<xml_diff>
--- a/LCA/LCI_ Inventories_NPi_2035.xlsx
+++ b/LCA/LCI_ Inventories_NPi_2035.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://listlu-my.sharepoint.com/personal/david_clousier_list_lu/Documents/Desktop/PAW/PAW_MFA_LCA_2025/LCA/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\welkerm\cursor\PAW_MFA_LCA_2025\LCA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{4A9171F6-1887-4FA1-B13E-31491570E266}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7C22D410-35CA-45B6-ACDA-D891947FAF69}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5392FFF9-15C9-4A57-B571-AFF3C4C88933}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{EF6BAC2F-8532-4D6B-ADAB-847A45F05723}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="13890" activeTab="1" xr2:uid="{EF6BAC2F-8532-4D6B-ADAB-847A45F05723}"/>
   </bookViews>
   <sheets>
     <sheet name="Directory" sheetId="2" r:id="rId1"/>
@@ -21,23 +21,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1164" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1162" uniqueCount="165">
   <si>
     <t>Database</t>
   </si>
@@ -399,9 +388,6 @@
     <t>market for transport, freight, lorry, unspecified</t>
   </si>
   <si>
-    <t>paw_db</t>
-  </si>
-  <si>
     <t>ecoinvent-3.11-biosphere</t>
   </si>
   <si>
@@ -532,13 +518,16 @@
   </si>
   <si>
     <t>ei_cutoff_3.11_remind-eu_SSP2-NPi_2035 2025-11-12</t>
+  </si>
+  <si>
+    <t>paw_NPi_2035</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -644,7 +633,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -982,14 +971,14 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.875" defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="15">
       <c r="A4" s="6">
         <v>230</v>
       </c>
@@ -997,7 +986,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="15">
       <c r="A5" s="8">
         <v>102</v>
       </c>
@@ -1005,7 +994,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="15">
       <c r="A6" s="7">
         <v>128</v>
       </c>
@@ -1023,18 +1012,18 @@
   <dimension ref="A1:O257"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E252" sqref="E252"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.875" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="26.109375" customWidth="1"/>
+    <col min="1" max="1" width="26.125" customWidth="1"/>
     <col min="2" max="2" width="34" customWidth="1"/>
-    <col min="8" max="8" width="15.109375" customWidth="1"/>
-    <col min="9" max="9" width="21.109375" customWidth="1"/>
+    <col min="8" max="8" width="15.125" customWidth="1"/>
+    <col min="9" max="9" width="21.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1042,15 +1031,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" s="4" customFormat="1" ht="15">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -1058,7 +1047,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
@@ -1066,7 +1055,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1074,7 +1063,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1082,7 +1071,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -1090,7 +1079,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1098,7 +1087,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1106,7 +1095,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1114,7 +1103,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -1122,7 +1111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -1130,7 +1119,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1138,7 +1127,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -1146,12 +1135,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -1198,7 +1187,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -1213,7 +1202,7 @@
       </c>
       <c r="E18" t="str">
         <f>$B$2</f>
-        <v>paw_db</v>
+        <v>paw_NPi_2035</v>
       </c>
       <c r="F18" t="s">
         <v>34</v>
@@ -1246,12 +1235,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15">
       <c r="A19" t="s">
         <v>36</v>
       </c>
       <c r="B19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C19">
         <v>0.23100000000000001</v>
@@ -1260,13 +1249,13 @@
         <v>40</v>
       </c>
       <c r="E19" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F19" t="s">
         <v>41</v>
       </c>
       <c r="G19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H19" t="s">
         <v>42</v>
@@ -1293,7 +1282,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15">
       <c r="A21" s="4" t="s">
         <v>8</v>
       </c>
@@ -1301,7 +1290,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -1309,7 +1298,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -1317,7 +1306,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15">
       <c r="A24" t="s">
         <v>11</v>
       </c>
@@ -1325,7 +1314,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -1333,7 +1322,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15">
       <c r="A26" t="s">
         <v>14</v>
       </c>
@@ -1341,7 +1330,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15">
       <c r="A27" t="s">
         <v>15</v>
       </c>
@@ -1349,7 +1338,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15">
       <c r="A28" t="s">
         <v>17</v>
       </c>
@@ -1357,7 +1346,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15">
       <c r="A29" t="s">
         <v>18</v>
       </c>
@@ -1365,7 +1354,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15">
       <c r="A30" t="s">
         <v>20</v>
       </c>
@@ -1373,7 +1362,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:15">
       <c r="A31" t="s">
         <v>22</v>
       </c>
@@ -1381,12 +1370,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:15">
       <c r="A32" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:15">
       <c r="A33" t="s">
         <v>9</v>
       </c>
@@ -1433,7 +1422,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:15">
       <c r="A34" t="s">
         <v>45</v>
       </c>
@@ -1448,7 +1437,7 @@
       </c>
       <c r="E34" t="str">
         <f>$B$2</f>
-        <v>paw_db</v>
+        <v>paw_NPi_2035</v>
       </c>
       <c r="F34" t="s">
         <v>34</v>
@@ -1481,7 +1470,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:15">
       <c r="A35" t="s">
         <v>36</v>
       </c>
@@ -1495,7 +1484,7 @@
         <v>48</v>
       </c>
       <c r="E35" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F35" t="s">
         <v>41</v>
@@ -1528,7 +1517,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:15">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -1542,7 +1531,7 @@
         <v>48</v>
       </c>
       <c r="E36" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F36" t="s">
         <v>41</v>
@@ -1575,7 +1564,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:15">
       <c r="A38" s="4" t="s">
         <v>8</v>
       </c>
@@ -1583,7 +1572,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:15">
       <c r="A39" t="s">
         <v>9</v>
       </c>
@@ -1591,7 +1580,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:15">
       <c r="A40" t="s">
         <v>10</v>
       </c>
@@ -1599,7 +1588,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:15">
       <c r="A41" t="s">
         <v>11</v>
       </c>
@@ -1607,7 +1596,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:15">
       <c r="A42" t="s">
         <v>12</v>
       </c>
@@ -1615,7 +1604,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:15">
       <c r="A43" t="s">
         <v>14</v>
       </c>
@@ -1623,7 +1612,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:15">
       <c r="A44" t="s">
         <v>15</v>
       </c>
@@ -1631,7 +1620,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:15">
       <c r="A45" t="s">
         <v>17</v>
       </c>
@@ -1639,7 +1628,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:15">
       <c r="A46" t="s">
         <v>18</v>
       </c>
@@ -1647,7 +1636,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:15">
       <c r="A47" t="s">
         <v>20</v>
       </c>
@@ -1655,7 +1644,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:15">
       <c r="A48" t="s">
         <v>22</v>
       </c>
@@ -1663,12 +1652,12 @@
         <v>54</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:15">
       <c r="A49" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:15">
       <c r="A50" t="s">
         <v>9</v>
       </c>
@@ -1715,7 +1704,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:15">
       <c r="A51" t="s">
         <v>53</v>
       </c>
@@ -1730,7 +1719,7 @@
       </c>
       <c r="E51" t="str">
         <f>$B$2</f>
-        <v>paw_db</v>
+        <v>paw_NPi_2035</v>
       </c>
       <c r="F51" t="s">
         <v>34</v>
@@ -1763,7 +1752,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:15">
       <c r="A52" t="s">
         <v>36</v>
       </c>
@@ -1777,7 +1766,7 @@
         <v>48</v>
       </c>
       <c r="E52" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F52" t="s">
         <v>41</v>
@@ -1810,7 +1799,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:15">
       <c r="A53" t="s">
         <v>36</v>
       </c>
@@ -1824,7 +1813,7 @@
         <v>48</v>
       </c>
       <c r="E53" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F53" t="s">
         <v>41</v>
@@ -1857,7 +1846,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:15">
       <c r="A54" t="s">
         <v>36</v>
       </c>
@@ -1871,7 +1860,7 @@
         <v>48</v>
       </c>
       <c r="E54" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F54" t="s">
         <v>41</v>
@@ -1904,7 +1893,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:15">
       <c r="A55" t="s">
         <v>36</v>
       </c>
@@ -1918,7 +1907,7 @@
         <v>48</v>
       </c>
       <c r="E55" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F55" t="s">
         <v>41</v>
@@ -1951,7 +1940,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:15">
       <c r="A56" t="s">
         <v>36</v>
       </c>
@@ -1965,7 +1954,7 @@
         <v>48</v>
       </c>
       <c r="E56" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F56" t="s">
         <v>41</v>
@@ -1998,7 +1987,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:15">
       <c r="A57" t="s">
         <v>36</v>
       </c>
@@ -2012,7 +2001,7 @@
         <v>48</v>
       </c>
       <c r="E57" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F57" t="s">
         <v>41</v>
@@ -2045,7 +2034,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:15">
       <c r="A58" t="s">
         <v>36</v>
       </c>
@@ -2059,7 +2048,7 @@
         <v>48</v>
       </c>
       <c r="E58" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F58" t="s">
         <v>41</v>
@@ -2092,7 +2081,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:15">
       <c r="A59" t="s">
         <v>36</v>
       </c>
@@ -2106,7 +2095,7 @@
         <v>48</v>
       </c>
       <c r="E59" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F59" t="s">
         <v>41</v>
@@ -2139,7 +2128,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:15">
       <c r="A60" t="s">
         <v>36</v>
       </c>
@@ -2153,7 +2142,7 @@
         <v>48</v>
       </c>
       <c r="E60" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F60" t="s">
         <v>41</v>
@@ -2186,7 +2175,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:15">
       <c r="A61" t="s">
         <v>36</v>
       </c>
@@ -2200,7 +2189,7 @@
         <v>48</v>
       </c>
       <c r="E61" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F61" t="s">
         <v>41</v>
@@ -2233,7 +2222,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:15">
       <c r="A62" t="s">
         <v>36</v>
       </c>
@@ -2247,7 +2236,7 @@
         <v>48</v>
       </c>
       <c r="E62" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F62" t="s">
         <v>41</v>
@@ -2280,7 +2269,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:15">
       <c r="A63" t="s">
         <v>36</v>
       </c>
@@ -2294,7 +2283,7 @@
         <v>48</v>
       </c>
       <c r="E63" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F63" t="s">
         <v>41</v>
@@ -2327,7 +2316,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:15">
       <c r="A64" t="s">
         <v>36</v>
       </c>
@@ -2341,7 +2330,7 @@
         <v>48</v>
       </c>
       <c r="E64" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F64" t="s">
         <v>41</v>
@@ -2374,7 +2363,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:15">
       <c r="A65" t="s">
         <v>36</v>
       </c>
@@ -2388,7 +2377,7 @@
         <v>48</v>
       </c>
       <c r="E65" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F65" t="s">
         <v>41</v>
@@ -2421,7 +2410,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:15">
       <c r="A66" t="s">
         <v>36</v>
       </c>
@@ -2435,7 +2424,7 @@
         <v>48</v>
       </c>
       <c r="E66" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F66" t="s">
         <v>41</v>
@@ -2468,7 +2457,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:15">
       <c r="A67" t="s">
         <v>36</v>
       </c>
@@ -2482,7 +2471,7 @@
         <v>48</v>
       </c>
       <c r="E67" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F67" t="s">
         <v>41</v>
@@ -2515,7 +2504,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:15">
       <c r="A68" t="s">
         <v>36</v>
       </c>
@@ -2529,7 +2518,7 @@
         <v>48</v>
       </c>
       <c r="E68" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F68" t="s">
         <v>41</v>
@@ -2562,7 +2551,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:15">
       <c r="A69" t="s">
         <v>36</v>
       </c>
@@ -2576,7 +2565,7 @@
         <v>48</v>
       </c>
       <c r="E69" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F69" t="s">
         <v>41</v>
@@ -2609,7 +2598,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:15">
       <c r="A71" s="4" t="s">
         <v>8</v>
       </c>
@@ -2617,7 +2606,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:15">
       <c r="A72" t="s">
         <v>9</v>
       </c>
@@ -2625,7 +2614,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:15">
       <c r="A73" t="s">
         <v>10</v>
       </c>
@@ -2633,7 +2622,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:15">
       <c r="A74" t="s">
         <v>11</v>
       </c>
@@ -2641,7 +2630,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:15">
       <c r="A75" t="s">
         <v>12</v>
       </c>
@@ -2649,7 +2638,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:15">
       <c r="A76" t="s">
         <v>14</v>
       </c>
@@ -2657,7 +2646,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:15">
       <c r="A77" t="s">
         <v>15</v>
       </c>
@@ -2665,7 +2654,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:15">
       <c r="A78" t="s">
         <v>17</v>
       </c>
@@ -2673,7 +2662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:15">
       <c r="A79" t="s">
         <v>18</v>
       </c>
@@ -2681,7 +2670,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:15">
       <c r="A80" t="s">
         <v>20</v>
       </c>
@@ -2689,7 +2678,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:15">
       <c r="A81" t="s">
         <v>22</v>
       </c>
@@ -2697,12 +2686,12 @@
         <v>92</v>
       </c>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:15">
       <c r="A82" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:15">
       <c r="A83" t="s">
         <v>9</v>
       </c>
@@ -2749,7 +2738,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:15">
       <c r="A84" t="s">
         <v>98</v>
       </c>
@@ -2764,7 +2753,7 @@
       </c>
       <c r="E84" t="str">
         <f>$B$2</f>
-        <v>paw_db</v>
+        <v>paw_NPi_2035</v>
       </c>
       <c r="F84" t="s">
         <v>34</v>
@@ -2797,7 +2786,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:15">
       <c r="A85" t="s">
         <v>36</v>
       </c>
@@ -2811,7 +2800,7 @@
         <v>48</v>
       </c>
       <c r="E85" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F85" t="s">
         <v>99</v>
@@ -2844,7 +2833,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:15">
       <c r="A86" t="s">
         <v>36</v>
       </c>
@@ -2858,7 +2847,7 @@
         <v>48</v>
       </c>
       <c r="E86" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F86" t="s">
         <v>41</v>
@@ -2891,7 +2880,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:15">
       <c r="A87" t="s">
         <v>36</v>
       </c>
@@ -2905,7 +2894,7 @@
         <v>21</v>
       </c>
       <c r="E87" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F87" t="s">
         <v>41</v>
@@ -2938,7 +2927,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:15">
       <c r="A88" t="s">
         <v>36</v>
       </c>
@@ -2952,7 +2941,7 @@
         <v>48</v>
       </c>
       <c r="E88" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F88" t="s">
         <v>41</v>
@@ -2985,31 +2974,31 @@
         <v>36</v>
       </c>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:15">
       <c r="A90" s="10" t="s">
         <v>8</v>
       </c>
       <c r="B90" s="10" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.3">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15">
       <c r="A91" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B91" s="10" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15">
+      <c r="A92" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="B92" s="10" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A92" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="B92" s="10" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:15">
       <c r="A93" t="s">
         <v>11</v>
       </c>
@@ -3017,15 +3006,15 @@
         <v>230</v>
       </c>
     </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:15">
       <c r="A94" t="s">
         <v>15</v>
       </c>
       <c r="B94" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="95" spans="1:15">
       <c r="A95" t="s">
         <v>17</v>
       </c>
@@ -3033,7 +3022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:15">
       <c r="A96" t="s">
         <v>18</v>
       </c>
@@ -3041,7 +3030,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:15">
       <c r="A97" t="s">
         <v>20</v>
       </c>
@@ -3049,7 +3038,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:15">
       <c r="A98" t="s">
         <v>22</v>
       </c>
@@ -3057,12 +3046,12 @@
         <v>102</v>
       </c>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:15">
       <c r="A99" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:15">
       <c r="A100" t="s">
         <v>9</v>
       </c>
@@ -3109,7 +3098,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:15">
       <c r="A101" t="str">
         <f>B91</f>
         <v>sec_tre =&gt; qua_tre__gac</v>
@@ -3127,7 +3116,7 @@
       </c>
       <c r="E101" t="str">
         <f>$B$2</f>
-        <v>paw_db</v>
+        <v>paw_NPi_2035</v>
       </c>
       <c r="F101" t="s">
         <v>34</v>
@@ -3162,7 +3151,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:15">
       <c r="A102" t="s">
         <v>36</v>
       </c>
@@ -3179,7 +3168,7 @@
       </c>
       <c r="E102" t="str">
         <f>E101</f>
-        <v>paw_db</v>
+        <v>paw_NPi_2035</v>
       </c>
       <c r="F102" t="s">
         <v>41</v>
@@ -3214,7 +3203,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:15">
       <c r="A103" t="s">
         <v>36</v>
       </c>
@@ -3231,7 +3220,7 @@
       </c>
       <c r="E103" t="str">
         <f>E102</f>
-        <v>paw_db</v>
+        <v>paw_NPi_2035</v>
       </c>
       <c r="F103" t="s">
         <v>34</v>
@@ -3266,7 +3255,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:15">
       <c r="A104" t="s">
         <v>36</v>
       </c>
@@ -3283,7 +3272,7 @@
       </c>
       <c r="E104" t="str">
         <f>E103</f>
-        <v>paw_db</v>
+        <v>paw_NPi_2035</v>
       </c>
       <c r="F104" t="s">
         <v>34</v>
@@ -3318,7 +3307,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:15">
       <c r="A105" t="s">
         <v>36</v>
       </c>
@@ -3335,7 +3324,7 @@
       </c>
       <c r="E105" t="str">
         <f>E104</f>
-        <v>paw_db</v>
+        <v>paw_NPi_2035</v>
       </c>
       <c r="F105" t="s">
         <v>34</v>
@@ -3370,7 +3359,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:15">
       <c r="A107" s="4" t="s">
         <v>8</v>
       </c>
@@ -3378,7 +3367,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:15">
       <c r="A108" t="s">
         <v>9</v>
       </c>
@@ -3386,7 +3375,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:15">
       <c r="A109" t="s">
         <v>10</v>
       </c>
@@ -3394,7 +3383,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:15">
       <c r="A110" t="s">
         <v>11</v>
       </c>
@@ -3402,7 +3391,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:15">
       <c r="A111" t="s">
         <v>12</v>
       </c>
@@ -3410,7 +3399,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:15">
       <c r="A112" t="s">
         <v>14</v>
       </c>
@@ -3418,7 +3407,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:15">
       <c r="A113" t="s">
         <v>15</v>
       </c>
@@ -3426,7 +3415,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:15">
       <c r="A114" t="s">
         <v>17</v>
       </c>
@@ -3434,7 +3423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:15">
       <c r="A115" t="s">
         <v>18</v>
       </c>
@@ -3442,7 +3431,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:15">
       <c r="A116" t="s">
         <v>20</v>
       </c>
@@ -3450,7 +3439,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:15">
       <c r="A117" t="s">
         <v>22</v>
       </c>
@@ -3458,12 +3447,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:15">
       <c r="A118" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:15">
       <c r="A119" t="s">
         <v>9</v>
       </c>
@@ -3510,7 +3499,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:15">
       <c r="A120" t="s">
         <v>105</v>
       </c>
@@ -3525,7 +3514,7 @@
       </c>
       <c r="E120" t="str">
         <f>$B$2</f>
-        <v>paw_db</v>
+        <v>paw_NPi_2035</v>
       </c>
       <c r="F120" t="s">
         <v>34</v>
@@ -3558,12 +3547,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:15">
       <c r="A121" t="s">
         <v>36</v>
       </c>
       <c r="B121" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C121">
         <v>0.17</v>
@@ -3572,13 +3561,13 @@
         <v>40</v>
       </c>
       <c r="E121" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F121" t="s">
         <v>34</v>
       </c>
       <c r="G121" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H121" t="s">
         <v>42</v>
@@ -3605,7 +3594,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:15">
       <c r="A123" s="4" t="s">
         <v>8</v>
       </c>
@@ -3613,7 +3602,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="124" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:15">
       <c r="A124" t="s">
         <v>9</v>
       </c>
@@ -3621,7 +3610,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="125" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:15">
       <c r="A125" t="s">
         <v>10</v>
       </c>
@@ -3629,7 +3618,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="126" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:15">
       <c r="A126" t="s">
         <v>11</v>
       </c>
@@ -3637,7 +3626,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="127" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:15">
       <c r="A127" t="s">
         <v>12</v>
       </c>
@@ -3645,7 +3634,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="128" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:15">
       <c r="A128" t="s">
         <v>14</v>
       </c>
@@ -3653,7 +3642,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="129" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:15">
       <c r="A129" t="s">
         <v>15</v>
       </c>
@@ -3661,7 +3650,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="130" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:15">
       <c r="A130" t="s">
         <v>17</v>
       </c>
@@ -3669,7 +3658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:15">
       <c r="A131" t="s">
         <v>18</v>
       </c>
@@ -3677,7 +3666,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="132" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:15">
       <c r="A132" t="s">
         <v>20</v>
       </c>
@@ -3685,7 +3674,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="133" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:15">
       <c r="A133" t="s">
         <v>22</v>
       </c>
@@ -3693,12 +3682,12 @@
         <v>54</v>
       </c>
     </row>
-    <row r="134" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:15">
       <c r="A134" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="135" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:15">
       <c r="A135" t="s">
         <v>9</v>
       </c>
@@ -3745,7 +3734,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="136" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:15">
       <c r="A136" t="s">
         <v>108</v>
       </c>
@@ -3760,7 +3749,7 @@
       </c>
       <c r="E136" t="str">
         <f>$B$2</f>
-        <v>paw_db</v>
+        <v>paw_NPi_2035</v>
       </c>
       <c r="F136" t="s">
         <v>34</v>
@@ -3793,7 +3782,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="137" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:15">
       <c r="A137" t="s">
         <v>36</v>
       </c>
@@ -3807,7 +3796,7 @@
         <v>48</v>
       </c>
       <c r="E137" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F137" t="s">
         <v>34</v>
@@ -3840,39 +3829,39 @@
         <v>36</v>
       </c>
     </row>
-    <row r="139" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:15" s="10" customFormat="1">
       <c r="A139" s="10" t="s">
         <v>8</v>
       </c>
       <c r="B139" s="10" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="140" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="140" spans="1:15" s="10" customFormat="1">
       <c r="A140" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B140" s="10" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="141" spans="1:15" s="10" customFormat="1">
+      <c r="A141" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="B141" s="10" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="141" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A141" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="B141" s="10" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="142" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:15">
       <c r="A142" t="s">
         <v>15</v>
       </c>
       <c r="B142" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="143" spans="1:15" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="143" spans="1:15">
       <c r="A143" t="s">
         <v>11</v>
       </c>
@@ -3880,7 +3869,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="144" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:15">
       <c r="A144" t="s">
         <v>17</v>
       </c>
@@ -3888,7 +3877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:15">
       <c r="A145" t="s">
         <v>18</v>
       </c>
@@ -3896,7 +3885,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="146" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:15">
       <c r="A146" t="s">
         <v>20</v>
       </c>
@@ -3904,20 +3893,20 @@
         <v>21</v>
       </c>
     </row>
-    <row r="147" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:15">
       <c r="A147" t="s">
         <v>22</v>
       </c>
       <c r="B147" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="148" spans="1:15" x14ac:dyDescent="0.3">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="148" spans="1:15">
       <c r="A148" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="149" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:15">
       <c r="A149" t="s">
         <v>9</v>
       </c>
@@ -3964,7 +3953,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="150" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:15">
       <c r="A150" t="str">
         <f>B140</f>
         <v>sec_tre =&gt; qua_tre__o3</v>
@@ -3982,7 +3971,7 @@
       </c>
       <c r="E150" t="str">
         <f>$B$2</f>
-        <v>paw_db</v>
+        <v>paw_NPi_2035</v>
       </c>
       <c r="F150" t="s">
         <v>34</v>
@@ -4017,7 +4006,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="151" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:15">
       <c r="A151" t="s">
         <v>36</v>
       </c>
@@ -4034,7 +4023,7 @@
       </c>
       <c r="E151" t="str">
         <f>E150</f>
-        <v>paw_db</v>
+        <v>paw_NPi_2035</v>
       </c>
       <c r="F151" t="s">
         <v>41</v>
@@ -4069,7 +4058,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="152" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:15">
       <c r="A152" t="s">
         <v>36</v>
       </c>
@@ -4086,7 +4075,7 @@
       </c>
       <c r="E152" t="str">
         <f>E151</f>
-        <v>paw_db</v>
+        <v>paw_NPi_2035</v>
       </c>
       <c r="F152" t="s">
         <v>34</v>
@@ -4122,32 +4111,32 @@
         <v>36</v>
       </c>
     </row>
-    <row r="153" spans="1:15" ht="13.65" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="154" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:15" ht="13.7" customHeight="1"/>
+    <row r="154" spans="1:15" s="10" customFormat="1">
       <c r="A154" s="10" t="s">
         <v>8</v>
       </c>
       <c r="B154" s="10" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="155" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="155" spans="1:15" s="10" customFormat="1">
       <c r="A155" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B155" s="10" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="156" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="156" spans="1:15" s="10" customFormat="1">
       <c r="A156" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B156" s="10" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="157" spans="1:15" x14ac:dyDescent="0.3">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="157" spans="1:15">
       <c r="A157" t="s">
         <v>10</v>
       </c>
@@ -4155,7 +4144,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="158" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:15">
       <c r="A158" t="s">
         <v>11</v>
       </c>
@@ -4163,7 +4152,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="159" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:15">
       <c r="A159" t="s">
         <v>12</v>
       </c>
@@ -4171,7 +4160,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="160" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:15">
       <c r="A160" t="s">
         <v>14</v>
       </c>
@@ -4179,15 +4168,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="161" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:15">
       <c r="A161" t="s">
         <v>15</v>
       </c>
       <c r="B161" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="162" spans="1:15" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="162" spans="1:15">
       <c r="A162" t="s">
         <v>17</v>
       </c>
@@ -4195,7 +4184,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:15">
       <c r="A163" t="s">
         <v>18</v>
       </c>
@@ -4203,7 +4192,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="164" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:15">
       <c r="A164" t="s">
         <v>20</v>
       </c>
@@ -4211,20 +4200,20 @@
         <v>21</v>
       </c>
     </row>
-    <row r="165" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:15">
       <c r="A165" t="s">
         <v>22</v>
       </c>
       <c r="B165" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="166" spans="1:15" x14ac:dyDescent="0.3">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="166" spans="1:15">
       <c r="A166" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="167" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:15">
       <c r="A167" t="s">
         <v>9</v>
       </c>
@@ -4271,7 +4260,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="168" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:15">
       <c r="A168" t="str">
         <f>B155</f>
         <v>sec_tre =&gt; qua_tre__aop</v>
@@ -4288,13 +4277,13 @@
       </c>
       <c r="E168" t="str">
         <f>$B$2</f>
-        <v>paw_db</v>
+        <v>paw_NPi_2035</v>
       </c>
       <c r="F168" t="s">
         <v>34</v>
       </c>
       <c r="G168" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H168" t="s">
         <v>35</v>
@@ -4322,7 +4311,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="169" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:15">
       <c r="A169" t="s">
         <v>36</v>
       </c>
@@ -4336,7 +4325,7 @@
         <v>48</v>
       </c>
       <c r="E169" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F169" t="s">
         <v>34</v>
@@ -4369,7 +4358,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="170" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:15">
       <c r="A170" t="s">
         <v>36</v>
       </c>
@@ -4383,7 +4372,7 @@
         <v>48</v>
       </c>
       <c r="E170" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F170" t="s">
         <v>34</v>
@@ -4416,7 +4405,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="171" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:15">
       <c r="A171" t="s">
         <v>36</v>
       </c>
@@ -4430,7 +4419,7 @@
         <v>48</v>
       </c>
       <c r="E171" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F171" t="s">
         <v>34</v>
@@ -4463,7 +4452,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="173" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:15" s="10" customFormat="1">
       <c r="A173" s="10" t="s">
         <v>8</v>
       </c>
@@ -4471,47 +4460,47 @@
         <v>112</v>
       </c>
     </row>
-    <row r="174" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:15" s="10" customFormat="1">
       <c r="A174" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B174" s="10" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="175" spans="1:15" s="10" customFormat="1">
+      <c r="A175" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="B175" s="10" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="175" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A175" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="B175" s="10" t="s">
+    <row r="176" spans="1:15" s="10" customFormat="1">
+      <c r="A176" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="B176" s="10" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="176" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A176" s="10" t="s">
+    <row r="177" spans="1:15" s="10" customFormat="1">
+      <c r="A177" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="B176" s="10" t="s">
+      <c r="B177" s="10" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="177" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A177" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="B177" s="10" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="178" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:15" s="10" customFormat="1">
       <c r="A178" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="B178" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="B178" s="10" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="179" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="179" spans="1:15">
       <c r="A179" t="s">
         <v>15</v>
       </c>
@@ -4519,7 +4508,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="180" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:15">
       <c r="A180" t="s">
         <v>17</v>
       </c>
@@ -4527,7 +4516,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:15">
       <c r="A181" t="s">
         <v>18</v>
       </c>
@@ -4535,7 +4524,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="182" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:15">
       <c r="A182" t="s">
         <v>20</v>
       </c>
@@ -4543,7 +4532,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="183" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:15">
       <c r="A183" t="s">
         <v>22</v>
       </c>
@@ -4551,12 +4540,12 @@
         <v>113</v>
       </c>
     </row>
-    <row r="184" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:15">
       <c r="A184" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="185" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:15">
       <c r="A185" t="s">
         <v>9</v>
       </c>
@@ -4603,7 +4592,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="186" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:15">
       <c r="A186" t="str">
         <f>B174</f>
         <v>qua_tre =&gt; inc__nof</v>
@@ -4621,7 +4610,7 @@
       </c>
       <c r="E186" t="str">
         <f>B2</f>
-        <v>paw_db</v>
+        <v>paw_NPi_2035</v>
       </c>
       <c r="F186" t="s">
         <v>34</v>
@@ -4656,7 +4645,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="187" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:15">
       <c r="A187" t="s">
         <v>36</v>
       </c>
@@ -4671,7 +4660,7 @@
         <v>kilogram</v>
       </c>
       <c r="E187" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F187" t="s">
         <v>41</v>
@@ -4705,8 +4694,8 @@
         <v>36</v>
       </c>
     </row>
-    <row r="188" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="189" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:15" ht="15.6" customHeight="1"/>
+    <row r="189" spans="1:15" s="10" customFormat="1">
       <c r="A189" s="10" t="s">
         <v>8</v>
       </c>
@@ -4714,47 +4703,47 @@
         <v>115</v>
       </c>
     </row>
-    <row r="190" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:15" s="10" customFormat="1">
       <c r="A190" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B190" s="10" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="191" spans="1:15" s="10" customFormat="1">
+      <c r="A191" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="B191" s="10" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="192" spans="1:15" s="10" customFormat="1">
+      <c r="A192" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="B192" s="10" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="191" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A191" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="B191" s="10" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="192" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A192" s="10" t="s">
+    <row r="193" spans="1:15" s="10" customFormat="1">
+      <c r="A193" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="B192" s="10" t="s">
+      <c r="B193" s="10" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="193" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A193" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="B193" s="10" t="s">
+    <row r="194" spans="1:15" s="10" customFormat="1">
+      <c r="A194" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="B194" s="10" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="194" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A194" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="B194" s="10" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="195" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:15">
       <c r="A195" t="s">
         <v>15</v>
       </c>
@@ -4762,7 +4751,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="196" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:15">
       <c r="A196" t="s">
         <v>17</v>
       </c>
@@ -4770,7 +4759,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:15">
       <c r="A197" t="s">
         <v>18</v>
       </c>
@@ -4778,7 +4767,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="198" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:15">
       <c r="A198" t="s">
         <v>20</v>
       </c>
@@ -4786,7 +4775,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="199" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:15">
       <c r="A199" t="s">
         <v>22</v>
       </c>
@@ -4794,12 +4783,12 @@
         <v>102</v>
       </c>
     </row>
-    <row r="200" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:15">
       <c r="A200" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="201" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:15">
       <c r="A201" t="s">
         <v>9</v>
       </c>
@@ -4846,7 +4835,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="202" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:15">
       <c r="A202" t="str">
         <f>B192</f>
         <v>dec_tre =&gt; sec_tre__o3</v>
@@ -4864,7 +4853,7 @@
       </c>
       <c r="E202" t="str">
         <f>$B$2</f>
-        <v>paw_db</v>
+        <v>paw_NPi_2035</v>
       </c>
       <c r="F202" t="s">
         <v>34</v>
@@ -4899,7 +4888,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="203" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:15">
       <c r="A203" t="s">
         <v>36</v>
       </c>
@@ -4914,7 +4903,7 @@
         <v>cubic meter</v>
       </c>
       <c r="E203" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F203" t="s">
         <v>41</v>
@@ -4949,7 +4938,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="205" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:15" s="10" customFormat="1">
       <c r="A205" s="10" t="s">
         <v>8</v>
       </c>
@@ -4957,55 +4946,55 @@
         <v>116</v>
       </c>
     </row>
-    <row r="206" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:15" s="10" customFormat="1">
       <c r="A206" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="B206" s="10" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="207" spans="1:15" s="10" customFormat="1">
+      <c r="A207" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="B207" s="10" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="208" spans="1:15" s="10" customFormat="1">
+      <c r="A208" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="B208" s="10" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="209" spans="1:15" s="10" customFormat="1">
+      <c r="A209" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="B209" s="10" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="210" spans="1:15" s="10" customFormat="1">
+      <c r="A210" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="B210" s="10" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="211" spans="1:15" s="10" customFormat="1">
+      <c r="A211" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="B211" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="B206" s="10" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="207" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A207" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="B207" s="10" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="208" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A208" s="10" t="s">
-        <v>148</v>
-      </c>
-      <c r="B208" s="10" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="209" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A209" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="B209" s="10" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="210" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A210" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="B210" s="10" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="211" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A211" s="10" t="s">
-        <v>163</v>
-      </c>
-      <c r="B211" s="10" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="212" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="212" spans="1:15">
       <c r="A212" t="s">
         <v>15</v>
       </c>
@@ -5013,7 +5002,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="213" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:15">
       <c r="A213" t="s">
         <v>17</v>
       </c>
@@ -5021,7 +5010,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="214" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:15">
       <c r="A214" t="s">
         <v>18</v>
       </c>
@@ -5029,15 +5018,15 @@
         <v>19</v>
       </c>
     </row>
-    <row r="215" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:15">
       <c r="A215" t="s">
         <v>20</v>
       </c>
       <c r="B215" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="216" spans="1:15" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="216" spans="1:15">
       <c r="A216" t="s">
         <v>22</v>
       </c>
@@ -5045,12 +5034,12 @@
         <v>117</v>
       </c>
     </row>
-    <row r="217" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:15">
       <c r="A217" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="218" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:15">
       <c r="A218" t="s">
         <v>9</v>
       </c>
@@ -5097,7 +5086,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="219" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:15">
       <c r="A219" t="str">
         <f>B211</f>
         <v>sldg_trans</v>
@@ -5115,7 +5104,7 @@
       </c>
       <c r="E219" t="str">
         <f>$B$2</f>
-        <v>paw_db</v>
+        <v>paw_NPi_2035</v>
       </c>
       <c r="F219" t="s">
         <v>34</v>
@@ -5150,7 +5139,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="220" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:15">
       <c r="A220" t="s">
         <v>36</v>
       </c>
@@ -5165,7 +5154,7 @@
         <v>ton kilometer</v>
       </c>
       <c r="E220" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F220" t="s">
         <v>41</v>
@@ -5199,7 +5188,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="222" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:15" s="10" customFormat="1">
       <c r="A222" s="10" t="s">
         <v>8</v>
       </c>
@@ -5207,15 +5196,15 @@
         <v>118</v>
       </c>
     </row>
-    <row r="223" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:15" s="10" customFormat="1">
       <c r="A223" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B223" s="10" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="224" spans="1:15" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="224" spans="1:15">
       <c r="A224" t="s">
         <v>15</v>
       </c>
@@ -5223,7 +5212,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="225" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:15">
       <c r="A225" t="s">
         <v>17</v>
       </c>
@@ -5231,7 +5220,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="226" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:15">
       <c r="A226" t="s">
         <v>18</v>
       </c>
@@ -5239,15 +5228,15 @@
         <v>19</v>
       </c>
     </row>
-    <row r="227" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:15">
       <c r="A227" t="s">
         <v>20</v>
       </c>
       <c r="B227" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="228" spans="1:15" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="228" spans="1:15">
       <c r="A228" t="s">
         <v>22</v>
       </c>
@@ -5255,12 +5244,12 @@
         <v>117</v>
       </c>
     </row>
-    <row r="229" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:15">
       <c r="A229" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="230" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:15">
       <c r="A230" t="s">
         <v>9</v>
       </c>
@@ -5307,7 +5296,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="231" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:15">
       <c r="A231" t="str">
         <f>B223</f>
         <v>fer =&gt; soi</v>
@@ -5325,7 +5314,7 @@
       </c>
       <c r="E231" t="str">
         <f>$B$2</f>
-        <v>paw_db</v>
+        <v>paw_NPi_2035</v>
       </c>
       <c r="F231" t="s">
         <v>34</v>
@@ -5360,7 +5349,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="232" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:15">
       <c r="A232" t="s">
         <v>36</v>
       </c>
@@ -5375,7 +5364,7 @@
         <v>ton kilometer</v>
       </c>
       <c r="E232" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F232" t="s">
         <v>41</v>
@@ -5409,31 +5398,31 @@
         <v>36</v>
       </c>
     </row>
-    <row r="234" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:15">
       <c r="A234" s="10" t="s">
         <v>8</v>
       </c>
       <c r="B234" s="10" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="235" spans="1:15" x14ac:dyDescent="0.3">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="235" spans="1:15">
       <c r="A235" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B235" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="236" spans="1:15">
+      <c r="A236" s="10" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="236" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A236" s="10" t="s">
-        <v>163</v>
-      </c>
       <c r="B236" s="10" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="237" spans="1:15" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="237" spans="1:15">
       <c r="A237" t="s">
         <v>15</v>
       </c>
@@ -5441,7 +5430,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="238" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:15">
       <c r="A238" t="s">
         <v>17</v>
       </c>
@@ -5449,7 +5438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="239" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:15">
       <c r="A239" t="s">
         <v>18</v>
       </c>
@@ -5457,7 +5446,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="240" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:15">
       <c r="A240" t="s">
         <v>20</v>
       </c>
@@ -5465,20 +5454,20 @@
         <v>48</v>
       </c>
     </row>
-    <row r="241" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:15">
       <c r="A241" t="s">
         <v>22</v>
       </c>
       <c r="B241" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="242" spans="1:15" x14ac:dyDescent="0.3">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="242" spans="1:15">
       <c r="A242" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="243" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:15">
       <c r="A243" t="s">
         <v>9</v>
       </c>
@@ -5525,9 +5514,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="244" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:15">
       <c r="A244" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B244" t="str">
         <f>B234</f>
@@ -5539,8 +5528,9 @@
       <c r="D244" t="s">
         <v>48</v>
       </c>
-      <c r="E244" t="s">
-        <v>120</v>
+      <c r="E244" t="str">
+        <f>B2</f>
+        <v>paw_NPi_2035</v>
       </c>
       <c r="F244" t="s">
         <v>34</v>
@@ -5574,9 +5564,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="245" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:15">
       <c r="B245" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C245">
         <v>1</v>
@@ -5585,32 +5575,32 @@
         <v>48</v>
       </c>
       <c r="E245" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F245" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H245" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="247" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:15">
       <c r="A247" s="10" t="s">
         <v>8</v>
       </c>
       <c r="B247" s="10" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="248" spans="1:15" x14ac:dyDescent="0.3">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="248" spans="1:15">
       <c r="A248" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B248" s="10" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="249" spans="1:15" x14ac:dyDescent="0.3">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="249" spans="1:15">
       <c r="A249" t="s">
         <v>15</v>
       </c>
@@ -5618,7 +5608,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="250" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:15">
       <c r="A250" t="s">
         <v>17</v>
       </c>
@@ -5626,7 +5616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="251" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:15">
       <c r="A251" t="s">
         <v>18</v>
       </c>
@@ -5634,7 +5624,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="252" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:15">
       <c r="A252" t="s">
         <v>20</v>
       </c>
@@ -5642,20 +5632,20 @@
         <v>48</v>
       </c>
     </row>
-    <row r="253" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:15">
       <c r="A253" t="s">
         <v>22</v>
       </c>
       <c r="B253" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="254" spans="1:15" x14ac:dyDescent="0.3">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="254" spans="1:15">
       <c r="A254" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="255" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:15">
       <c r="A255" t="s">
         <v>9</v>
       </c>
@@ -5702,9 +5692,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="256" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:15">
       <c r="A256" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B256" t="str">
         <f>B247</f>
@@ -5716,8 +5706,9 @@
       <c r="D256" t="s">
         <v>48</v>
       </c>
-      <c r="E256" t="s">
-        <v>120</v>
+      <c r="E256" t="str">
+        <f>B2</f>
+        <v>paw_NPi_2035</v>
       </c>
       <c r="F256" t="s">
         <v>34</v>
@@ -5751,9 +5742,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="257" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="257" spans="2:8">
       <c r="B257" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C257">
         <v>1</v>
@@ -5762,10 +5753,10 @@
         <v>48</v>
       </c>
       <c r="E257" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F257" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H257" t="s">
         <v>74</v>

</xml_diff>